<commit_message>
aggregating proportion.msm to state and msa
</commit_message>
<xml_diff>
--- a/documentation/Data Manager/outcomes/Surveillance Manager Data Overview_5.12.25 .xlsx
+++ b/documentation/Data Manager/outcomes/Surveillance Manager Data Overview_5.12.25 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/zdansky1_jh_edu/Documents/Documents/JHEEM/code/jheem_analyses/documentation/Data Manager/outcomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1481" documentId="8_{5B8C9924-F6D7-44DC-B572-4281B68F07E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BD92DA-A204-428D-9D5B-A21832533E68}"/>
+  <xr:revisionPtr revIDLastSave="1493" documentId="8_{5B8C9924-F6D7-44DC-B572-4281B68F07E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C36D0E1D-1010-42B5-AE90-F208A916EB56}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8579475C-7638-4116-B28E-AE987A3A13E6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="variance" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">estimates!$A$1:$L$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">estimates!$A$1:$L$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="296">
   <si>
     <t>Outcome</t>
   </si>
@@ -914,6 +914,18 @@
   </si>
   <si>
     <t>This is the denominator value for proprotion.msm</t>
+  </si>
+  <si>
+    <t>emory.aggregated</t>
+  </si>
+  <si>
+    <t>section.3.processing</t>
+  </si>
+  <si>
+    <t>Used pull function to aggregate data from county to MSA and state. Note that we are only aggregating data that we have so there may be counties missing from a state (in Alaska for example).</t>
+  </si>
+  <si>
+    <t>MSA; State</t>
   </si>
 </sst>
 </file>
@@ -1414,11 +1426,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9038165-BF80-43CF-98BC-A2B368BC0F5A}">
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5598,71 +5610,71 @@
         <v>191</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D116" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E116" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G116" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H116" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I116" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="J116" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="K116" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="L116" s="18"/>
+        <v>40</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E116" s="15">
+        <v>2013</v>
+      </c>
+      <c r="F116" t="s">
+        <v>111</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I116" t="s">
+        <v>293</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>191</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E117" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F117" t="s">
-        <v>96</v>
-      </c>
-      <c r="G117" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G117" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H117" s="3" t="s">
+      <c r="H117" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I117" t="s">
-        <v>233</v>
-      </c>
-      <c r="J117" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L117" s="21" t="s">
-        <v>271</v>
-      </c>
+      <c r="I117" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="J117" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K117" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="L117" s="18"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -5672,16 +5684,16 @@
         <v>41</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E118" s="15" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F118" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>104</v>
@@ -5695,15 +5707,50 @@
       <c r="J118" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="K118" t="s">
-        <v>115</v>
-      </c>
       <c r="L118" s="21" t="s">
         <v>271</v>
       </c>
     </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>191</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E119" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F119" t="s">
+        <v>114</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I119" t="s">
+        <v>233</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K119" t="s">
+        <v>115</v>
+      </c>
+      <c r="L119" s="21" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L119" xr:uid="{D9038165-BF80-43CF-98BC-A2B368BC0F5A}"/>
+  <autoFilter ref="A1:L120" xr:uid="{D9038165-BF80-43CF-98BC-A2B368BC0F5A}"/>
   <hyperlinks>
     <hyperlink ref="L65" r:id="rId1" xr:uid="{75C1ECF5-CC47-4810-BDE0-D9B7710BBCA9}"/>
     <hyperlink ref="L57" r:id="rId2" xr:uid="{72889D92-82B6-41B2-A34E-E60CD2AFB70C}"/>

</xml_diff>